<commit_message>
Update as per walkthrough
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MyComputer\Documents\UiPath\Advanced training\Client Security Hash\ClientSecurityHash_REF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277AD174-94CB-4FF1-A05E-7CFDA126CDAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CDE820-D187-4AC0-BD5D-A6FD1385E451}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -178,13 +178,31 @@
   </si>
   <si>
     <t>SecurityHashQueue</t>
+  </si>
+  <si>
+    <t>System_1_URL</t>
+  </si>
+  <si>
+    <t>SHA1_Online_URL</t>
+  </si>
+  <si>
+    <t>http://www.sha1-online.com</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com</t>
+  </si>
+  <si>
+    <t>The url for the ACME test site</t>
+  </si>
+  <si>
+    <t>The url for the hash generation site</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -194,6 +212,12 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -214,14 +238,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -537,7 +564,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -615,8 +642,28 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1609,8 +1656,12 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{C8DC7530-3295-4F3A-A517-8AFC3F640390}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{A4BF65E9-A49D-4EC0-99C9-59AAEA1BC52A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1618,7 +1669,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2831,7 +2884,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Initial update as per walkthrough
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MyComputer\Documents\UiPath\Advanced training\Client Security Hash\ClientSecurityHash_REF\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TNAGABA002\Documents\UiPath\Advanced training\Client Hash\client_security_hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CDE820-D187-4AC0-BD5D-A6FD1385E451}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48C704E-40D3-43CF-AA60-93A52F87FD68}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -564,7 +564,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>